<commit_message>
ADP Report and other changes
</commit_message>
<xml_diff>
--- a/ExcelTemplates/_Template - WOAnalysis_01 - MMM-MMM.xlsx
+++ b/ExcelTemplates/_Template - WOAnalysis_01 - MMM-MMM.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617AF329-A810-4767-909A-BC38379206D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEA15FC-CF38-4634-94C3-94EA4590CF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="401" xr2:uid="{3C759B79-F44A-4AB8-ADE2-0792C7E368A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="494" xr2:uid="{3C759B79-F44A-4AB8-ADE2-0792C7E368A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="3" r:id="rId1"/>
     <sheet name="Lookup Tables" sheetId="4" r:id="rId2"/>
     <sheet name="Results Explained" sheetId="6" r:id="rId3"/>
+    <sheet name="ADP Missing WO" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$BI$1</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="105">
   <si>
     <t>WONumber</t>
   </si>
@@ -279,186 +280,6 @@
     <t>InvoicePrice
 - (minus)
 SalesTax</t>
-  </si>
-  <si>
-    <t>Ambo</t>
-  </si>
-  <si>
-    <t>Nicholas</t>
-  </si>
-  <si>
-    <t>Bautista</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>BP Construction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camilo Ortiz  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yunior Alberto  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defranca  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luiz Humberto  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garcia De Los Santos  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cesar A.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gonzalez  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elena  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gonzalez </t>
-  </si>
-  <si>
-    <t>Alejandro</t>
-  </si>
-  <si>
-    <t>Hagan</t>
-  </si>
-  <si>
-    <t>Bernard J.</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Hagan Jr.</t>
-  </si>
-  <si>
-    <t>Bernard</t>
-  </si>
-  <si>
-    <t>Hill</t>
-  </si>
-  <si>
-    <t>Brandon J.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huchko  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joseph R.  </t>
-  </si>
-  <si>
-    <t>Lara Construction</t>
-  </si>
-  <si>
-    <t>Marte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Randy R  </t>
-  </si>
-  <si>
-    <t>Martinez Alba</t>
-  </si>
-  <si>
-    <t>Enmanual</t>
-  </si>
-  <si>
-    <t>Martinez Alba-50</t>
-  </si>
-  <si>
-    <t>Mcss Construction</t>
-  </si>
-  <si>
-    <t>Montanez</t>
-  </si>
-  <si>
-    <t>Jose L.</t>
-  </si>
-  <si>
-    <t>Negrette</t>
-  </si>
-  <si>
-    <t>Victor</t>
-  </si>
-  <si>
-    <t>Nunez</t>
-  </si>
-  <si>
-    <t>Angel</t>
-  </si>
-  <si>
-    <t>Ortega</t>
-  </si>
-  <si>
-    <t>Jorge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ortega Victoria  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jorge D  </t>
-  </si>
-  <si>
-    <t>Reyes</t>
-  </si>
-  <si>
-    <t>Alexis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rodriguez  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isabel  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justin J.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sepulveda Jr.  </t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torres  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wilfredo  </t>
-  </si>
-  <si>
-    <t>Vasquez</t>
-  </si>
-  <si>
-    <t>Joshua</t>
-  </si>
-  <si>
-    <t>Vicente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hector Jose  </t>
-  </si>
-  <si>
-    <t>LaborMarkup</t>
-  </si>
-  <si>
-    <t>Internal</t>
-  </si>
-  <si>
-    <t>Outside</t>
-  </si>
-  <si>
-    <t>MaterialMarkup</t>
-  </si>
-  <si>
-    <t>Oil</t>
-  </si>
-  <si>
-    <t>Repairs</t>
   </si>
   <si>
     <r>
@@ -840,36 +661,6 @@
     <t>KeyString2</t>
   </si>
   <si>
-    <t>APH-Boiler</t>
-  </si>
-  <si>
-    <t>APH-Plumbing</t>
-  </si>
-  <si>
-    <t>Plumbing</t>
-  </si>
-  <si>
-    <t>Supplies</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Boiler</t>
-  </si>
-  <si>
-    <t>Co-Op</t>
-  </si>
-  <si>
-    <t>Kitchen</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Paint</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Labor_Total
  x
@@ -963,16 +754,22 @@
     </r>
   </si>
   <si>
-    <t>Proposals</t>
+    <t>CompanyCode</t>
   </si>
   <si>
-    <t>Violation</t>
+    <t>PayrollName</t>
   </si>
   <si>
-    <t>AFP</t>
+    <t>FileNumber</t>
   </si>
   <si>
-    <t>Super</t>
+    <t>PayDate</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Dollars</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +876,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,6 +898,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1204,11 +1007,15 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1530,7 +1337,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY8" sqref="AY8"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1604,25 +1411,25 @@
         <v>5</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="H1" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="L1" s="22" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="N1" s="22" t="s">
         <v>8</v>
@@ -1640,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="S1" s="24" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="T1" s="25" t="s">
         <v>13</v>
@@ -1715,16 +1522,16 @@
         <v>36</v>
       </c>
       <c r="AR1" s="25" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="AS1" s="25" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="AT1" s="25" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="AU1" s="25" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="AV1" s="29" t="s">
         <v>37</v>
@@ -13189,10 +12996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A7EB70-D16E-4C28-8F83-46986E16FACE}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13211,20 +13018,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="H1" s="33" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="H1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -13253,812 +13060,27 @@
         <v>59</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="K2" s="27" t="s">
         <v>60</v>
       </c>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="11">
-        <v>160</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="11">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="K4" s="11">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="11">
-        <v>1.7</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K5" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="11">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="K6" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="11">
-        <v>90</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K7" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="11">
-        <v>100</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="K8" s="11">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="11">
-        <v>60</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K9" s="11">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="11">
-        <v>60</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K10" s="11">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="11">
-        <v>100</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>25</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K11" s="11">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="11">
-        <v>160</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="K12" s="11">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="11">
-        <v>90</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="K13" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="11">
-        <v>30</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="K14" s="11">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="11">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>30</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="K15" s="11">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="11">
-        <v>47</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="K16" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="11">
-        <v>1.7</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="K17" s="11">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C18" s="11">
-        <v>100</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K18" s="11">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="11">
-        <v>40</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="K19" s="11">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="11">
-        <v>50</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="J20" s="34" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="11">
-        <v>1.7</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="11">
-        <v>50</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>35</v>
-      </c>
-      <c r="J22" s="34" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="11">
-        <v>40</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="J23" s="34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="11">
-        <v>100</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="J24" s="34" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="11">
-        <v>50</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="11">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="11">
-        <v>100</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="11">
-        <v>40</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="11">
-        <v>15</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="11">
-        <v>60</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="11">
-        <v>60</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="11">
-        <v>40</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" s="11">
-        <v>50</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
+    <row r="20" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J21" s="33"/>
+    </row>
+    <row r="22" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J22" s="33"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J23" s="33"/>
+    </row>
+    <row r="24" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J24" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -14074,9 +13096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1498219D-D660-4818-BE53-0290365DFDFE}">
   <dimension ref="A1:BI1435"/>
   <sheetViews>
-    <sheetView topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="AZ2" sqref="AZ2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14146,19 +13166,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="L1" s="18" t="s">
         <v>7</v>
@@ -14182,7 +13202,7 @@
         <v>12</v>
       </c>
       <c r="S1" s="20" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="T1" s="19" t="s">
         <v>13</v>
@@ -14257,16 +13277,16 @@
         <v>36</v>
       </c>
       <c r="AR1" s="19" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="AS1" s="19" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="AT1" s="19" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="AU1" s="19" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="AV1" s="18" t="s">
         <v>37</v>
@@ -14316,11 +13336,11 @@
         <v>64</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="14" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16" t="s">
@@ -14328,35 +13348,35 @@
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="16" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="U2" s="14" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="X2" s="14" t="s">
         <v>62</v>
       </c>
       <c r="Z2" s="15"/>
       <c r="AA2" s="14" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="AR2" s="9"/>
       <c r="AS2" s="9"/>
@@ -14366,32 +13386,32 @@
         <v>66</v>
       </c>
       <c r="AZ2" s="14" t="s">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="BA2" s="14" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="BB2" s="17" t="s">
         <v>67</v>
       </c>
       <c r="BC2" s="17"/>
       <c r="BD2" s="17" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="BE2" s="17" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="BF2" s="17" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="BG2" s="17" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="BH2" s="17" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="BI2" s="17" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.3">
@@ -27546,4 +26566,1162 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB36317-9EE1-4828-B190-E2586744561E}">
+  <dimension ref="A1:G371"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="36" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" s="35"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="35"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="35"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" s="35"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="35"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="35"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="35"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" s="35"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="35"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="35"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="35"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="35"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="35"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="35"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="35"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="35"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="35"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="35"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="35"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="35"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E31" s="35"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="35"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="35"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="35"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="35"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="35"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="35"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="35"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="35"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="35"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="35"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E43" s="35"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="35"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="35"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="35"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="35"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="35"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="35"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="35"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="35"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="35"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E53" s="35"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E54" s="35"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E55" s="35"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E56" s="35"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E57" s="35"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E58" s="35"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E59" s="35"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E60" s="35"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E61" s="35"/>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E62" s="35"/>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E63" s="35"/>
+    </row>
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E64" s="35"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="35"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="35"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E67" s="35"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E68" s="35"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="35"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E70" s="35"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E71" s="35"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E72" s="35"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E73" s="35"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E74" s="35"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E75" s="35"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E76" s="35"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E77" s="35"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E78" s="35"/>
+    </row>
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E79" s="35"/>
+    </row>
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E80" s="35"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E81" s="35"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E82" s="35"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E83" s="35"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E84" s="35"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E85" s="35"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E86" s="35"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E87" s="35"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E88" s="35"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E89" s="35"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E90" s="35"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E91" s="35"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E92" s="35"/>
+    </row>
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E93" s="35"/>
+    </row>
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E94" s="35"/>
+    </row>
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E95" s="35"/>
+    </row>
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E96" s="35"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E97" s="35"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E98" s="35"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E99" s="35"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E100" s="35"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E101" s="35"/>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E102" s="35"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E103" s="35"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E104" s="35"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E105" s="35"/>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E106" s="35"/>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E107" s="35"/>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E108" s="35"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E109" s="35"/>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E110" s="35"/>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E111" s="35"/>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E112" s="35"/>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E113" s="35"/>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E114" s="35"/>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E115" s="35"/>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E116" s="35"/>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E117" s="35"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E118" s="35"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E119" s="35"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E120" s="35"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E121" s="35"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E122" s="35"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E123" s="35"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E124" s="35"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E125" s="35"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E126" s="35"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E127" s="35"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E128" s="35"/>
+    </row>
+    <row r="129" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E129" s="35"/>
+    </row>
+    <row r="130" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E130" s="35"/>
+    </row>
+    <row r="131" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E131" s="35"/>
+    </row>
+    <row r="132" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E132" s="35"/>
+    </row>
+    <row r="133" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E133" s="35"/>
+    </row>
+    <row r="134" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E134" s="35"/>
+    </row>
+    <row r="135" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E135" s="35"/>
+    </row>
+    <row r="136" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E136" s="35"/>
+    </row>
+    <row r="137" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E137" s="35"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E138" s="35"/>
+    </row>
+    <row r="139" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E139" s="35"/>
+    </row>
+    <row r="140" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E140" s="35"/>
+    </row>
+    <row r="141" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E141" s="35"/>
+    </row>
+    <row r="142" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E142" s="35"/>
+    </row>
+    <row r="143" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E143" s="35"/>
+    </row>
+    <row r="144" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E144" s="35"/>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E145" s="35"/>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E146" s="35"/>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E147" s="35"/>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E148" s="35"/>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E149" s="35"/>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E150" s="35"/>
+    </row>
+    <row r="151" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E151" s="35"/>
+    </row>
+    <row r="152" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E152" s="35"/>
+    </row>
+    <row r="153" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E153" s="35"/>
+    </row>
+    <row r="154" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E154" s="35"/>
+    </row>
+    <row r="155" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E155" s="35"/>
+    </row>
+    <row r="156" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E156" s="35"/>
+    </row>
+    <row r="157" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E157" s="35"/>
+    </row>
+    <row r="158" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E158" s="35"/>
+    </row>
+    <row r="159" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E159" s="35"/>
+    </row>
+    <row r="160" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E160" s="35"/>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E161" s="35"/>
+    </row>
+    <row r="162" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E162" s="35"/>
+    </row>
+    <row r="163" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E163" s="35"/>
+    </row>
+    <row r="164" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E164" s="35"/>
+    </row>
+    <row r="165" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E165" s="35"/>
+    </row>
+    <row r="166" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E166" s="35"/>
+    </row>
+    <row r="167" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E167" s="35"/>
+    </row>
+    <row r="168" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E168" s="35"/>
+    </row>
+    <row r="169" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E169" s="35"/>
+    </row>
+    <row r="170" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E170" s="35"/>
+    </row>
+    <row r="171" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E171" s="35"/>
+    </row>
+    <row r="172" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E172" s="35"/>
+    </row>
+    <row r="173" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E173" s="35"/>
+    </row>
+    <row r="174" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E174" s="35"/>
+    </row>
+    <row r="175" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E175" s="35"/>
+    </row>
+    <row r="176" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E176" s="35"/>
+    </row>
+    <row r="177" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E177" s="35"/>
+    </row>
+    <row r="178" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E178" s="35"/>
+    </row>
+    <row r="179" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E179" s="35"/>
+    </row>
+    <row r="180" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E180" s="35"/>
+    </row>
+    <row r="181" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E181" s="35"/>
+    </row>
+    <row r="182" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E182" s="35"/>
+    </row>
+    <row r="183" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E183" s="35"/>
+    </row>
+    <row r="184" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E184" s="35"/>
+    </row>
+    <row r="185" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E185" s="35"/>
+    </row>
+    <row r="186" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E186" s="35"/>
+    </row>
+    <row r="187" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E187" s="35"/>
+    </row>
+    <row r="188" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E188" s="35"/>
+    </row>
+    <row r="189" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E189" s="35"/>
+    </row>
+    <row r="190" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E190" s="35"/>
+    </row>
+    <row r="191" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E191" s="35"/>
+    </row>
+    <row r="192" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E192" s="35"/>
+    </row>
+    <row r="193" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E193" s="35"/>
+    </row>
+    <row r="194" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E194" s="35"/>
+    </row>
+    <row r="195" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E195" s="35"/>
+    </row>
+    <row r="196" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E196" s="35"/>
+    </row>
+    <row r="197" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E197" s="35"/>
+    </row>
+    <row r="198" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E198" s="35"/>
+    </row>
+    <row r="199" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E199" s="35"/>
+    </row>
+    <row r="200" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E200" s="35"/>
+    </row>
+    <row r="201" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E201" s="35"/>
+    </row>
+    <row r="202" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E202" s="35"/>
+    </row>
+    <row r="203" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E203" s="35"/>
+    </row>
+    <row r="204" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E204" s="35"/>
+    </row>
+    <row r="205" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E205" s="35"/>
+    </row>
+    <row r="206" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E206" s="35"/>
+    </row>
+    <row r="207" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E207" s="35"/>
+    </row>
+    <row r="208" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E208" s="35"/>
+    </row>
+    <row r="209" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E209" s="35"/>
+    </row>
+    <row r="210" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E210" s="35"/>
+    </row>
+    <row r="211" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E211" s="35"/>
+    </row>
+    <row r="212" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E212" s="35"/>
+    </row>
+    <row r="213" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E213" s="35"/>
+    </row>
+    <row r="214" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E214" s="35"/>
+    </row>
+    <row r="215" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E215" s="35"/>
+    </row>
+    <row r="216" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E216" s="35"/>
+    </row>
+    <row r="217" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E217" s="35"/>
+    </row>
+    <row r="218" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E218" s="35"/>
+    </row>
+    <row r="219" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E219" s="35"/>
+    </row>
+    <row r="220" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E220" s="35"/>
+    </row>
+    <row r="221" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E221" s="35"/>
+    </row>
+    <row r="222" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E222" s="35"/>
+    </row>
+    <row r="223" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E223" s="35"/>
+    </row>
+    <row r="224" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E224" s="35"/>
+    </row>
+    <row r="225" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E225" s="35"/>
+    </row>
+    <row r="226" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E226" s="35"/>
+    </row>
+    <row r="227" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E227" s="35"/>
+    </row>
+    <row r="228" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E228" s="35"/>
+    </row>
+    <row r="229" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E229" s="35"/>
+    </row>
+    <row r="230" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E230" s="35"/>
+    </row>
+    <row r="231" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E231" s="35"/>
+    </row>
+    <row r="232" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E232" s="35"/>
+    </row>
+    <row r="233" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E233" s="35"/>
+    </row>
+    <row r="234" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E234" s="35"/>
+    </row>
+    <row r="235" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E235" s="35"/>
+    </row>
+    <row r="236" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E236" s="35"/>
+    </row>
+    <row r="237" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E237" s="35"/>
+    </row>
+    <row r="238" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E238" s="35"/>
+    </row>
+    <row r="239" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E239" s="35"/>
+    </row>
+    <row r="240" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E240" s="35"/>
+    </row>
+    <row r="241" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E241" s="35"/>
+    </row>
+    <row r="242" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E242" s="35"/>
+    </row>
+    <row r="243" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E243" s="35"/>
+    </row>
+    <row r="244" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E244" s="35"/>
+    </row>
+    <row r="245" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E245" s="35"/>
+    </row>
+    <row r="246" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E246" s="35"/>
+    </row>
+    <row r="247" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E247" s="35"/>
+    </row>
+    <row r="248" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E248" s="35"/>
+    </row>
+    <row r="249" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E249" s="35"/>
+    </row>
+    <row r="250" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E250" s="35"/>
+    </row>
+    <row r="251" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E251" s="35"/>
+    </row>
+    <row r="252" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E252" s="35"/>
+    </row>
+    <row r="253" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E253" s="35"/>
+    </row>
+    <row r="254" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E254" s="35"/>
+    </row>
+    <row r="255" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E255" s="35"/>
+    </row>
+    <row r="256" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E256" s="35"/>
+    </row>
+    <row r="257" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E257" s="35"/>
+    </row>
+    <row r="258" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E258" s="35"/>
+    </row>
+    <row r="259" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E259" s="35"/>
+    </row>
+    <row r="260" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E260" s="35"/>
+    </row>
+    <row r="261" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E261" s="35"/>
+    </row>
+    <row r="262" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E262" s="35"/>
+    </row>
+    <row r="263" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E263" s="35"/>
+    </row>
+    <row r="264" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E264" s="35"/>
+    </row>
+    <row r="265" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E265" s="35"/>
+    </row>
+    <row r="266" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E266" s="35"/>
+    </row>
+    <row r="267" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E267" s="35"/>
+    </row>
+    <row r="268" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E268" s="35"/>
+    </row>
+    <row r="269" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E269" s="35"/>
+    </row>
+    <row r="270" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E270" s="35"/>
+    </row>
+    <row r="271" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E271" s="35"/>
+    </row>
+    <row r="272" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E272" s="35"/>
+    </row>
+    <row r="273" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E273" s="35"/>
+    </row>
+    <row r="274" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E274" s="35"/>
+    </row>
+    <row r="275" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E275" s="35"/>
+    </row>
+    <row r="276" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E276" s="35"/>
+    </row>
+    <row r="277" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E277" s="35"/>
+    </row>
+    <row r="278" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E278" s="35"/>
+    </row>
+    <row r="279" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E279" s="35"/>
+    </row>
+    <row r="280" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E280" s="35"/>
+    </row>
+    <row r="281" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E281" s="35"/>
+    </row>
+    <row r="282" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E282" s="35"/>
+    </row>
+    <row r="283" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E283" s="35"/>
+    </row>
+    <row r="284" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E284" s="35"/>
+    </row>
+    <row r="285" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E285" s="35"/>
+    </row>
+    <row r="286" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E286" s="35"/>
+    </row>
+    <row r="287" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E287" s="35"/>
+    </row>
+    <row r="288" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E288" s="35"/>
+    </row>
+    <row r="289" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E289" s="35"/>
+    </row>
+    <row r="290" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E290" s="35"/>
+    </row>
+    <row r="291" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E291" s="35"/>
+    </row>
+    <row r="292" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E292" s="35"/>
+    </row>
+    <row r="293" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E293" s="35"/>
+    </row>
+    <row r="294" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E294" s="35"/>
+    </row>
+    <row r="295" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E295" s="35"/>
+    </row>
+    <row r="296" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E296" s="35"/>
+    </row>
+    <row r="297" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E297" s="35"/>
+    </row>
+    <row r="298" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E298" s="35"/>
+    </row>
+    <row r="299" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E299" s="35"/>
+    </row>
+    <row r="300" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E300" s="35"/>
+    </row>
+    <row r="301" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E301" s="35"/>
+    </row>
+    <row r="302" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E302" s="35"/>
+    </row>
+    <row r="303" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E303" s="35"/>
+    </row>
+    <row r="304" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E304" s="35"/>
+    </row>
+    <row r="305" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E305" s="35"/>
+    </row>
+    <row r="306" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E306" s="35"/>
+    </row>
+    <row r="307" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E307" s="35"/>
+    </row>
+    <row r="308" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E308" s="35"/>
+    </row>
+    <row r="309" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E309" s="35"/>
+    </row>
+    <row r="310" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E310" s="35"/>
+    </row>
+    <row r="311" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E311" s="35"/>
+    </row>
+    <row r="312" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E312" s="35"/>
+    </row>
+    <row r="313" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E313" s="35"/>
+    </row>
+    <row r="314" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E314" s="35"/>
+    </row>
+    <row r="315" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E315" s="35"/>
+    </row>
+    <row r="316" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E316" s="35"/>
+    </row>
+    <row r="317" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E317" s="35"/>
+    </row>
+    <row r="318" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E318" s="35"/>
+    </row>
+    <row r="319" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E319" s="35"/>
+    </row>
+    <row r="320" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E320" s="35"/>
+    </row>
+    <row r="321" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E321" s="35"/>
+    </row>
+    <row r="322" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E322" s="35"/>
+    </row>
+    <row r="323" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E323" s="35"/>
+    </row>
+    <row r="324" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E324" s="35"/>
+    </row>
+    <row r="325" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E325" s="35"/>
+    </row>
+    <row r="326" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E326" s="35"/>
+    </row>
+    <row r="327" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E327" s="35"/>
+    </row>
+    <row r="328" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E328" s="35"/>
+    </row>
+    <row r="329" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E329" s="35"/>
+    </row>
+    <row r="330" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E330" s="35"/>
+    </row>
+    <row r="331" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E331" s="35"/>
+    </row>
+    <row r="332" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E332" s="35"/>
+    </row>
+    <row r="333" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E333" s="35"/>
+    </row>
+    <row r="334" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E334" s="35"/>
+    </row>
+    <row r="335" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E335" s="35"/>
+    </row>
+    <row r="336" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E336" s="35"/>
+    </row>
+    <row r="337" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E337" s="35"/>
+    </row>
+    <row r="338" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E338" s="35"/>
+    </row>
+    <row r="339" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E339" s="35"/>
+    </row>
+    <row r="340" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E340" s="35"/>
+    </row>
+    <row r="341" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E341" s="35"/>
+    </row>
+    <row r="342" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E342" s="35"/>
+    </row>
+    <row r="343" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E343" s="35"/>
+    </row>
+    <row r="344" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E344" s="35"/>
+    </row>
+    <row r="345" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E345" s="35"/>
+    </row>
+    <row r="346" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E346" s="35"/>
+    </row>
+    <row r="347" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E347" s="35"/>
+    </row>
+    <row r="348" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E348" s="35"/>
+    </row>
+    <row r="349" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E349" s="35"/>
+    </row>
+    <row r="350" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E350" s="35"/>
+    </row>
+    <row r="351" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E351" s="35"/>
+    </row>
+    <row r="352" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E352" s="35"/>
+    </row>
+    <row r="353" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E353" s="35"/>
+    </row>
+    <row r="354" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E354" s="35"/>
+    </row>
+    <row r="355" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E355" s="35"/>
+    </row>
+    <row r="356" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E356" s="35"/>
+    </row>
+    <row r="357" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E357" s="35"/>
+    </row>
+    <row r="358" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E358" s="35"/>
+    </row>
+    <row r="359" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E359" s="35"/>
+    </row>
+    <row r="360" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E360" s="35"/>
+    </row>
+    <row r="361" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E361" s="35"/>
+    </row>
+    <row r="362" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E362" s="35"/>
+    </row>
+    <row r="363" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E363" s="35"/>
+    </row>
+    <row r="364" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E364" s="35"/>
+    </row>
+    <row r="365" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E365" s="35"/>
+    </row>
+    <row r="366" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E366" s="35"/>
+    </row>
+    <row r="367" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E367" s="35"/>
+    </row>
+    <row r="368" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E368" s="35"/>
+    </row>
+    <row r="369" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E369" s="35"/>
+    </row>
+    <row r="370" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E370" s="35"/>
+    </row>
+    <row r="371" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E371" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>